<commit_message>
updated age column to remove dollar sign and change salaries less than 20k
</commit_message>
<xml_diff>
--- a/renameDF.xlsx
+++ b/renameDF.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,46 +589,42 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Eve</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D5" t="n">
-        <v>1000000</v>
+        <v>100460</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2016-10-17</t>
+          <t>2022-08-19</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Marketing</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Late submissions</t>
-        </is>
-      </c>
+          <t>Sales</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.33/1</t>
+        </is>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -636,16 +632,14 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>37</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>$100460</t>
-        </is>
+        <v>49</v>
+      </c>
+      <c r="D6" t="n">
+        <v>65316.93</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2022-08-19</t>
+          <t>2019-09-26</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -653,71 +647,69 @@
           <t>Sales</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>0.33/1</t>
-        </is>
+      <c r="G6" t="n">
+        <v>0.73</v>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Promoted</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>Charlie</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D7" t="n">
-        <v>65316.93</v>
+        <v>65317.26</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2019-09-26</t>
+          <t>2021-09-08</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Sales</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>0.73</v>
+        <v>0.64</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Promoted</t>
-        </is>
-      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Charlie</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D8" t="n">
-        <v>65317.26</v>
+        <v>101584.26</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2021-09-08</t>
+          <t>2015-09-18</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -725,9 +717,7 @@
           <t>HR</t>
         </is>
       </c>
-      <c r="G8" t="n">
-        <v>0.64</v>
-      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" t="b">
         <v>0</v>
       </c>
@@ -735,143 +725,147 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bob</t>
+          <t>Hank</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D9" t="n">
-        <v>101584.26</v>
+        <v>85348</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2015-09-18</t>
+          <t>2018/13/01</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>HR</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" t="inlineStr"/>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>0.47</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Late submissions</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Hank</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>30</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>$85348</t>
-        </is>
+        <v>43</v>
+      </c>
+      <c r="D10" t="n">
+        <v>60610.51</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2018/13/01</t>
+          <t>2019-04-26</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Sales</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>0.47</v>
-      </c>
-      <c r="H10" t="inlineStr"/>
+        <v>0.12</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Late submissions</t>
+          <t>Promoted</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bob</t>
+          <t>Ivy</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" t="n">
-        <v>60610.51</v>
+        <v>80851</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>2019-04-26</t>
+          <t>2019-04-13</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Sales</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+        <v>0.71</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Promoted</t>
+          <t>Late submissions</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ivy</t>
+          <t>Grace</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>42</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>$80851</t>
-        </is>
+        <v>33</v>
+      </c>
+      <c r="D12" t="n">
+        <v>85359.98</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2019-04-13</t>
+          <t>2021-09-06</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Sales</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="H12" t="b">
-        <v>0</v>
+        <v>0.76</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -881,74 +875,64 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Grace</t>
+          <t>Alice</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2021-09-06</t>
-        </is>
-      </c>
+        <v>60685.4</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
           <t>Sales</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Late submissions</t>
-        </is>
-      </c>
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Grace</t>
+          <t>Alice</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D14" t="n">
-        <v>5</v>
+        <v>74839.25</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2021-09-06</t>
+          <t>2020-04-01</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Sales</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>0.76</v>
+        <v>0.77</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -959,158 +943,166 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Alice</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D15" t="n">
-        <v>60685.4</v>
-      </c>
-      <c r="E15" t="inlineStr"/>
+        <v>31734.4</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2020-12-07</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr">
         <is>
           <t>Sales</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="H15" t="b">
-        <v>0</v>
+        <v>0.49</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
       <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Alice</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D16" t="n">
-        <v>74839.25</v>
+        <v>35501.64</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2020-04-01</t>
+          <t>2018/13/01</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>0.77</v>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>Late submissions</t>
-        </is>
-      </c>
+        <v>0.52</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Bob</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D17" t="n">
-        <v>31734.4</v>
+        <v>58754.25</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>2020-12-07</t>
+          <t>2017-10-26</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Sales</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr"/>
+        <v>0.43</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Late submissions</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>Hank</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D18" t="n">
-        <v>35501.64</v>
+        <v>49743.38</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2018/13/01</t>
+          <t>2021-03-16</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="H18" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" t="inlineStr"/>
+        <v>0.03</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Late submissions</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>Ivy</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="D19" t="n">
-        <v>58754.25</v>
+        <v>76284.95</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2017-10-26</t>
+          <t>2015-02-17</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1119,11 +1111,9 @@
         </is>
       </c>
       <c r="G19" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
+        <v>0.11</v>
+      </c>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
           <t>Late submissions</t>
@@ -1132,118 +1122,116 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Hank</t>
+          <t>Alice</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="D20" t="n">
-        <v>49743.38</v>
+        <v>51839.52</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2021-03-16</t>
+          <t>2022-08-18</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="G20" t="n">
         <v>0.03</v>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+      <c r="H20" t="b">
+        <v>1</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Late submissions</t>
+          <t>On leave</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Ivy</t>
+          <t>Hank</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D21" t="n">
-        <v>76284.95</v>
+        <v>41753.93</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2015-02-17</t>
+          <t>2023-01-31</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="H21" t="inlineStr"/>
+        <v>0.64</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Late submissions</t>
+          <t>On leave</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Alice</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D22" t="n">
-        <v>51839.52</v>
+        <v>250000</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2022-08-18</t>
+          <t>2016-04-14</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="H22" t="b">
-        <v>1</v>
-      </c>
+        <v>0.31</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr">
         <is>
-          <t>On leave</t>
+          <t>Promoted</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1251,23 +1239,23 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="D23" t="n">
-        <v>41753.93</v>
+        <v>65484.47</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2023-01-31</t>
+          <t>2018/13/01</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>0.64</v>
+        <v>0.51</v>
       </c>
       <c r="H23" t="b">
         <v>1</v>
@@ -1280,33 +1268,31 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>Grace</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D24" t="n">
-        <v>250000</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>2016-04-14</t>
-        </is>
-      </c>
+        <v>71350.56</v>
+      </c>
+      <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="H24" t="inlineStr"/>
+        <v>0.91</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
       <c r="I24" t="inlineStr">
         <is>
           <t>Promoted</t>
@@ -1315,34 +1301,34 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Hank</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="D25" t="n">
-        <v>65484.47</v>
+        <v>41505.04</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>2018/13/01</t>
+          <t>2022-08-24</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>0.51</v>
+        <v>0.25</v>
       </c>
       <c r="H25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -1352,55 +1338,55 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Grace</t>
+          <t>Jarel</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D26" t="n">
-        <v>71350.56</v>
-      </c>
-      <c r="E26" t="inlineStr"/>
+        <v>59112.35</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2021-01-08</t>
+        </is>
+      </c>
       <c r="F26" t="inlineStr">
         <is>
           <t>HR</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>0.91</v>
+        <v>0.41</v>
       </c>
       <c r="H26" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>Promoted</t>
-        </is>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>Ivy</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="D27" t="n">
-        <v>41505.04</v>
+        <v>72218.45</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2022-08-24</t>
+          <t>2017-12-28</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1409,121 +1395,123 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="H27" t="b">
-        <v>0</v>
+        <v>0.76</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>On leave</t>
+          <t>Promoted</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Jarel</t>
+          <t>Eve</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D28" t="n">
-        <v>59112.35</v>
+        <v>46980.13</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2021-01-08</t>
+          <t>2022-03-10</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="H28" t="b">
-        <v>0</v>
-      </c>
-      <c r="I28" t="inlineStr"/>
+        <v>0.23</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>On leave</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Ivy</t>
+          <t>Alice</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D29" t="n">
-        <v>72218.45</v>
+        <v>77513.96000000001</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>2017-12-28</t>
+          <t>2018-10-25</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Sales</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>0.76</v>
+        <v>0.08</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
           <t>False</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>Promoted</t>
-        </is>
-      </c>
+      <c r="I29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Eve</t>
+          <t>Charlie</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D30" t="n">
-        <v>46980.13</v>
+        <v>57987.23</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>2022-03-10</t>
+          <t>2018/13/01</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+        <v>0.29</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -1533,31 +1521,31 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Alice</t>
+          <t>Grace</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D31" t="n">
-        <v>77513.96000000001</v>
+        <v>64166.13</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>2018-10-25</t>
+          <t>2016-04-01</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Sales</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -1568,94 +1556,88 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Charlie</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="D32" t="n">
-        <v>57987.23</v>
+        <v>57965.87</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>2018/13/01</t>
+          <t>2018-04-17</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Sales</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>0.29</v>
+        <v>0.93</v>
       </c>
       <c r="H32" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>On leave</t>
-        </is>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Grace</t>
+          <t>Eve</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D33" t="n">
-        <v>64166.13</v>
+        <v>107045.56</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2016-04-01</t>
+          <t>2019-11-16</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
       </c>
       <c r="I33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Charlie</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D34" t="n">
-        <v>57965.87</v>
+        <v>69730.06</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2018-04-17</t>
+          <t>2016-10-09</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1664,171 +1646,179 @@
         </is>
       </c>
       <c r="G34" t="n">
-        <v>0.93</v>
-      </c>
-      <c r="H34" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" t="inlineStr"/>
+        <v>0.63</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Late submissions</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Eve</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D35" t="n">
-        <v>107045.56</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>2019-11-16</t>
-        </is>
-      </c>
+        <v>48845.78</v>
+      </c>
+      <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.87</v>
       </c>
       <c r="H35" t="b">
-        <v>0</v>
-      </c>
-      <c r="I35" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Late submissions</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Charlie</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="D36" t="n">
-        <v>69730.06</v>
+        <v>86450.89999999999</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>2016-10-09</t>
+          <t>2020-02-02</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Sales</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>0.63</v>
+        <v>0.8</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
           <t>False</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>Late submissions</t>
-        </is>
-      </c>
+      <c r="I36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D37" t="n">
-        <v>48845.78</v>
-      </c>
-      <c r="E37" t="inlineStr"/>
+        <v>45583.13</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2018/13/01</t>
+        </is>
+      </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Sales</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>0.87</v>
-      </c>
-      <c r="H37" t="b">
-        <v>1</v>
-      </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>Late submissions</t>
-        </is>
-      </c>
+        <v>0.19</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="D38" t="n">
-        <v>86450.89999999999</v>
+        <v>74177.27</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>2020-02-02</t>
+          <t>2015-01-14</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Sales</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>0.8</v>
+        <v>0.89</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
           <t>False</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Late submissions</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Bob</t>
+          <t>Grace</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D39" t="n">
-        <v>45583.13</v>
+        <v>30806.6</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>2018/13/01</t>
+          <t>2023-02-05</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1837,18 +1827,22 @@
         </is>
       </c>
       <c r="G39" t="n">
-        <v>0.19</v>
+        <v>0.54</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
           <t>True</t>
         </is>
       </c>
-      <c r="I39" t="inlineStr"/>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Promoted</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1856,23 +1850,23 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="D40" t="n">
-        <v>74177.27</v>
+        <v>43436.28</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2015-01-14</t>
+          <t>2023-01-26</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Sales</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>0.89</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
@@ -1887,22 +1881,22 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Grace</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D41" t="n">
-        <v>30806.6</v>
+        <v>73937.22</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>2023-02-05</t>
+          <t>2017-12-14</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1911,46 +1905,42 @@
         </is>
       </c>
       <c r="G41" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
-      </c>
+        <v>0.9</v>
+      </c>
+      <c r="H41" t="inlineStr"/>
       <c r="I41" t="inlineStr">
         <is>
-          <t>Promoted</t>
+          <t>On leave</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Bob</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="D42" t="n">
-        <v>43436.28</v>
+        <v>84769.33</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>2023-01-26</t>
+          <t>2020-08-12</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Sales</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.32</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
@@ -1959,39 +1949,39 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Late submissions</t>
+          <t>Promoted</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Ivy</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D43" t="n">
-        <v>73937.22</v>
+        <v>73427.37</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>2017-12-14</t>
+          <t>2017-01-01</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Sales</t>
-        </is>
-      </c>
-      <c r="G43" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H43" t="inlineStr"/>
+          <t>HR</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="b">
+        <v>0</v>
+      </c>
       <c r="I43" t="inlineStr">
         <is>
           <t>On leave</t>
@@ -2000,22 +1990,22 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Eve</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="D44" t="n">
-        <v>84769.33</v>
+        <v>67687.03</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>2020-08-12</t>
+          <t>2018/13/01</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -2024,201 +2014,195 @@
         </is>
       </c>
       <c r="G44" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>Promoted</t>
-        </is>
-      </c>
+        <v>0.23</v>
+      </c>
+      <c r="H44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Ivy</t>
+          <t>Alice</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D45" t="n">
-        <v>73427.37</v>
+        <v>63977.93</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>2017-01-01</t>
+          <t>2020-09-10</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>HR</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="b">
-        <v>0</v>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>0.43/1</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>On leave</t>
+          <t>Promoted</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Sammy</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
         <v>43</v>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Eve</t>
-        </is>
-      </c>
-      <c r="C46" t="n">
-        <v>51</v>
-      </c>
       <c r="D46" t="n">
-        <v>67687.03</v>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>2018/13/01</t>
-        </is>
-      </c>
+        <v>40429.56</v>
+      </c>
+      <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Sales</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>0.23</v>
+        <v>0.82</v>
       </c>
       <c r="H46" t="b">
         <v>0</v>
       </c>
-      <c r="I46" t="inlineStr"/>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>On leave</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Alice</t>
+          <t>Hank</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D47" t="n">
-        <v>63977.93</v>
+        <v>55603.12</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2020-09-10</t>
+          <t>2016-03-11</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>0.43/1</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="H47" t="b">
+        <v>1</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>Promoted</t>
+          <t>On leave</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Sammy</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D48" t="n">
-        <v>40429.56</v>
-      </c>
-      <c r="E48" t="inlineStr"/>
+        <v>60787.22</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2022-01-05</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>HR</t>
-        </is>
-      </c>
-      <c r="G48" t="n">
-        <v>0.82</v>
-      </c>
-      <c r="H48" t="b">
-        <v>0</v>
-      </c>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>0.01/1</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr"/>
       <c r="I48" t="inlineStr">
         <is>
-          <t>On leave</t>
+          <t>Promoted</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Hank</t>
+          <t>Grace</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D49" t="n">
-        <v>55603.12</v>
+        <v>91142.44</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>2016-03-11</t>
+          <t>2018-05-07</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="H49" t="b">
-        <v>1</v>
-      </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>On leave</t>
-        </is>
-      </c>
+        <v>0.51</v>
+      </c>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -2226,51 +2210,51 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D50" t="n">
-        <v>60787.22</v>
+        <v>76872</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2022-01-05</t>
+          <t>2022-03-02</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>0.01/1</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr"/>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="H50" t="b">
+        <v>1</v>
+      </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Promoted</t>
+          <t>Late submissions</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Grace</t>
+          <t>Hank</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D51" t="n">
-        <v>91142.44</v>
+        <v>34739.2</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>2018-05-07</t>
+          <t>2018/13/01</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -2279,31 +2263,37 @@
         </is>
       </c>
       <c r="G51" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="inlineStr"/>
+        <v>0.22</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>On leave</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Bob</t>
+          <t>Eve</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>28</v>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>$76872</t>
-        </is>
+        <v>55</v>
+      </c>
+      <c r="D52" t="n">
+        <v>76481.67999999999</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2022-03-02</t>
+          <t>2020-09-10</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -2312,7 +2302,7 @@
         </is>
       </c>
       <c r="G52" t="n">
-        <v>0.42</v>
+        <v>0.12</v>
       </c>
       <c r="H52" t="b">
         <v>1</v>
@@ -2325,83 +2315,75 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Hank</t>
+          <t>Ivy</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="D53" t="n">
-        <v>34739.2</v>
+        <v>62298.35</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2018/13/01</t>
+          <t>2021-10-30</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>True</t>
-        </is>
+        <v>0.34</v>
+      </c>
+      <c r="H53" t="b">
+        <v>1</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>On leave</t>
+          <t>Late submissions</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Eve</t>
+          <t>Frank</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="D54" t="n">
-        <v>76481.67999999999</v>
+        <v>56461.56</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>2020-09-10</t>
+          <t>2017-03-25</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="G54" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="H54" t="b">
-        <v>1</v>
-      </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>Late submissions</t>
-        </is>
-      </c>
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -2409,26 +2391,28 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D55" t="n">
-        <v>62298.35</v>
+        <v>82233.53</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>2021-10-30</t>
+          <t>2016-09-18</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Sales</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="H55" t="b">
-        <v>1</v>
+        <v>0.32</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
@@ -2438,195 +2422,191 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D56" t="n">
-        <v>56461.56</v>
+        <v>90619.99000000001</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2017-03-25</t>
+          <t>2019-03-12</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Sales</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.52</v>
       </c>
       <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>On leave</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Ivy</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="C57" t="n">
         <v>57</v>
       </c>
       <c r="D57" t="n">
-        <v>82233.53</v>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>2016-09-18</t>
-        </is>
-      </c>
+        <v>88625</v>
+      </c>
+      <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Sales</t>
-        </is>
-      </c>
-      <c r="G57" t="n">
-        <v>0.32</v>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>Late submissions</t>
-        </is>
-      </c>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>0.7/1</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>Alice</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D58" t="n">
-        <v>90619.99000000001</v>
+        <v>53215.65</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>2019-03-12</t>
+          <t>2018/13/01</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Sales</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="H58" t="inlineStr"/>
+        <v>0.36</v>
+      </c>
+      <c r="H58" t="b">
+        <v>0</v>
+      </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>On leave</t>
+          <t>Promoted</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Bob</t>
+          <t>Diana</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>57</v>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>$88625</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr"/>
+        <v>43</v>
+      </c>
+      <c r="D59" t="n">
+        <v>63815.75</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2016-10-23</t>
+        </is>
+      </c>
       <c r="F59" t="inlineStr">
         <is>
           <t>Marketing</t>
         </is>
       </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>0.7/1</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr"/>
+      <c r="G59" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="H59" t="b">
+        <v>1</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>On leave</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Alice</t>
+          <t>Eve</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="D60" t="n">
-        <v>53215.65</v>
+        <v>76625.27</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>2018/13/01</t>
+          <t>2021-01-18</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>HR</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="H60" t="b">
-        <v>0</v>
-      </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>Promoted</t>
-        </is>
-      </c>
+        <v>0.96</v>
+      </c>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Diana</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D61" t="n">
-        <v>63815.75</v>
+        <v>89510.89999999999</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>2016-10-23</t>
+          <t>2020-12-12</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2635,80 +2615,12 @@
         </is>
       </c>
       <c r="G61" t="n">
-        <v>0.97</v>
+        <v>0.25</v>
       </c>
       <c r="H61" t="b">
         <v>1</v>
       </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>On leave</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>59</v>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Eve</t>
-        </is>
-      </c>
-      <c r="C62" t="n">
-        <v>34</v>
-      </c>
-      <c r="D62" t="n">
-        <v>76625.27</v>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>2021-01-18</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>Marketing</t>
-        </is>
-      </c>
-      <c r="G62" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="H62" t="inlineStr"/>
-      <c r="I62" t="inlineStr"/>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>60</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Bob</t>
-        </is>
-      </c>
-      <c r="C63" t="n">
-        <v>28</v>
-      </c>
-      <c r="D63" t="n">
-        <v>89510.89999999999</v>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>2020-12-12</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>Marketing</t>
-        </is>
-      </c>
-      <c r="G63" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="H63" t="b">
-        <v>1</v>
-      </c>
-      <c r="I63" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated data types and inconsistent fields with respective columns
</commit_message>
<xml_diff>
--- a/renameDF.xlsx
+++ b/renameDF.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -495,7 +499,9 @@
       <c r="D2" t="n">
         <v>79934.28</v>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" s="2" t="n">
+        <v>35886</v>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>Sales</t>
@@ -528,10 +534,8 @@
       <c r="D3" t="n">
         <v>67234.71000000001</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2022-01-14</t>
-        </is>
+      <c r="E3" s="2" t="n">
+        <v>44575</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -563,10 +567,8 @@
       <c r="D4" t="n">
         <v>1000000</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2016-10-17</t>
-        </is>
+      <c r="E4" s="2" t="n">
+        <v>42660</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -602,20 +604,16 @@
       <c r="D5" t="n">
         <v>100460</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>2022-08-19</t>
-        </is>
+      <c r="E5" s="2" t="n">
+        <v>44792</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>Sales</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>0.33/1</t>
-        </is>
+      <c r="G5" t="n">
+        <v>0.33</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
@@ -637,10 +635,8 @@
       <c r="D6" t="n">
         <v>65316.93</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2019-09-26</t>
-        </is>
+      <c r="E6" s="2" t="n">
+        <v>43734</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -674,10 +670,8 @@
       <c r="D7" t="n">
         <v>65317.26</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>2021-09-08</t>
-        </is>
+      <c r="E7" s="2" t="n">
+        <v>44447</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -707,17 +701,17 @@
       <c r="D8" t="n">
         <v>101584.26</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2015-09-18</t>
-        </is>
+      <c r="E8" s="2" t="n">
+        <v>42265</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>HR</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>0.68</v>
+      </c>
       <c r="H8" t="b">
         <v>0</v>
       </c>
@@ -738,10 +732,8 @@
       <c r="D9" t="n">
         <v>85348</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2018/13/01</t>
-        </is>
+      <c r="E9" s="2" t="n">
+        <v>40940</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -751,7 +743,9 @@
       <c r="G9" t="n">
         <v>0.47</v>
       </c>
-      <c r="H9" t="inlineStr"/>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
       <c r="I9" t="inlineStr">
         <is>
           <t>Late submissions</t>
@@ -773,10 +767,8 @@
       <c r="D10" t="n">
         <v>60610.51</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>2019-04-26</t>
-        </is>
+      <c r="E10" s="2" t="n">
+        <v>43581</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -812,10 +804,8 @@
       <c r="D11" t="n">
         <v>80851</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2019-04-13</t>
-        </is>
+      <c r="E11" s="2" t="n">
+        <v>43568</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -849,10 +839,8 @@
       <c r="D12" t="n">
         <v>85359.98</v>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2021-09-06</t>
-        </is>
+      <c r="E12" s="2" t="n">
+        <v>44445</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -888,7 +876,9 @@
       <c r="D13" t="n">
         <v>60685.4</v>
       </c>
-      <c r="E13" t="inlineStr"/>
+      <c r="E13" s="2" t="n">
+        <v>36495</v>
+      </c>
       <c r="F13" t="inlineStr">
         <is>
           <t>Sales</t>
@@ -917,10 +907,8 @@
       <c r="D14" t="n">
         <v>74839.25</v>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2020-04-01</t>
-        </is>
+      <c r="E14" s="2" t="n">
+        <v>43922</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -956,10 +944,8 @@
       <c r="D15" t="n">
         <v>31734.4</v>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2020-12-07</t>
-        </is>
+      <c r="E15" s="2" t="n">
+        <v>44172</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -991,10 +977,8 @@
       <c r="D16" t="n">
         <v>35501.64</v>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2018/13/01</t>
-        </is>
+      <c r="E16" s="2" t="n">
+        <v>40940</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1024,10 +1008,8 @@
       <c r="D17" t="n">
         <v>58754.25</v>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2017-10-26</t>
-        </is>
+      <c r="E17" s="2" t="n">
+        <v>43034</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1061,10 +1043,8 @@
       <c r="D18" t="n">
         <v>49743.38</v>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2021-03-16</t>
-        </is>
+      <c r="E18" s="2" t="n">
+        <v>44271</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1100,10 +1080,8 @@
       <c r="D19" t="n">
         <v>76284.95</v>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2015-02-17</t>
-        </is>
+      <c r="E19" s="2" t="n">
+        <v>42052</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1113,7 +1091,9 @@
       <c r="G19" t="n">
         <v>0.11</v>
       </c>
-      <c r="H19" t="inlineStr"/>
+      <c r="H19" t="b">
+        <v>1</v>
+      </c>
       <c r="I19" t="inlineStr">
         <is>
           <t>Late submissions</t>
@@ -1135,10 +1115,8 @@
       <c r="D20" t="n">
         <v>51839.52</v>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>2022-08-18</t>
-        </is>
+      <c r="E20" s="2" t="n">
+        <v>44791</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1172,10 +1150,8 @@
       <c r="D21" t="n">
         <v>41753.93</v>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>2023-01-31</t>
-        </is>
+      <c r="E21" s="2" t="n">
+        <v>44957</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1209,10 +1185,8 @@
       <c r="D22" t="n">
         <v>250000</v>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>2016-04-14</t>
-        </is>
+      <c r="E22" s="2" t="n">
+        <v>42474</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1222,7 +1196,9 @@
       <c r="G22" t="n">
         <v>0.31</v>
       </c>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
       <c r="I22" t="inlineStr">
         <is>
           <t>Promoted</t>
@@ -1244,10 +1220,8 @@
       <c r="D23" t="n">
         <v>65484.47</v>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>2018/13/01</t>
-        </is>
+      <c r="E23" s="2" t="n">
+        <v>40940</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1281,7 +1255,9 @@
       <c r="D24" t="n">
         <v>71350.56</v>
       </c>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" s="2" t="n">
+        <v>38867</v>
+      </c>
       <c r="F24" t="inlineStr">
         <is>
           <t>HR</t>
@@ -1314,10 +1290,8 @@
       <c r="D25" t="n">
         <v>41505.04</v>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>2022-08-24</t>
-        </is>
+      <c r="E25" s="2" t="n">
+        <v>44797</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1351,10 +1325,8 @@
       <c r="D26" t="n">
         <v>59112.35</v>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>2021-01-08</t>
-        </is>
+      <c r="E26" s="2" t="n">
+        <v>44204</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1384,10 +1356,8 @@
       <c r="D27" t="n">
         <v>72218.45</v>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>2017-12-28</t>
-        </is>
+      <c r="E27" s="2" t="n">
+        <v>43097</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1423,10 +1393,8 @@
       <c r="D28" t="n">
         <v>46980.13</v>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>2022-03-10</t>
-        </is>
+      <c r="E28" s="2" t="n">
+        <v>44630</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1462,10 +1430,8 @@
       <c r="D29" t="n">
         <v>77513.96000000001</v>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>2018-10-25</t>
-        </is>
+      <c r="E29" s="2" t="n">
+        <v>43398</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1497,10 +1463,8 @@
       <c r="D30" t="n">
         <v>57987.23</v>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>2018/13/01</t>
-        </is>
+      <c r="E30" s="2" t="n">
+        <v>40940</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1534,10 +1498,8 @@
       <c r="D31" t="n">
         <v>64166.13</v>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>2016-04-01</t>
-        </is>
+      <c r="E31" s="2" t="n">
+        <v>42461</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1569,10 +1531,8 @@
       <c r="D32" t="n">
         <v>57965.87</v>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>2018-04-17</t>
-        </is>
+      <c r="E32" s="2" t="n">
+        <v>43207</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1602,10 +1562,8 @@
       <c r="D33" t="n">
         <v>107045.56</v>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>2019-11-16</t>
-        </is>
+      <c r="E33" s="2" t="n">
+        <v>43785</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1635,10 +1593,8 @@
       <c r="D34" t="n">
         <v>69730.06</v>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>2016-10-09</t>
-        </is>
+      <c r="E34" s="2" t="n">
+        <v>42652</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1674,7 +1630,9 @@
       <c r="D35" t="n">
         <v>48845.78</v>
       </c>
-      <c r="E35" t="inlineStr"/>
+      <c r="E35" s="2" t="n">
+        <v>45930</v>
+      </c>
       <c r="F35" t="inlineStr">
         <is>
           <t>Engineering</t>
@@ -1707,10 +1665,8 @@
       <c r="D36" t="n">
         <v>86450.89999999999</v>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>2020-02-02</t>
-        </is>
+      <c r="E36" s="2" t="n">
+        <v>43863</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1718,7 +1674,7 @@
         </is>
       </c>
       <c r="G36" t="n">
-        <v>0.8</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
@@ -1742,10 +1698,8 @@
       <c r="D37" t="n">
         <v>45583.13</v>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>2018/13/01</t>
-        </is>
+      <c r="E37" s="2" t="n">
+        <v>41483</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1777,10 +1731,8 @@
       <c r="D38" t="n">
         <v>74177.27</v>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>2015-01-14</t>
-        </is>
+      <c r="E38" s="2" t="n">
+        <v>42018</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1816,10 +1768,8 @@
       <c r="D39" t="n">
         <v>30806.6</v>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>2023-02-05</t>
-        </is>
+      <c r="E39" s="2" t="n">
+        <v>44962</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1855,10 +1805,8 @@
       <c r="D40" t="n">
         <v>43436.28</v>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>2023-01-26</t>
-        </is>
+      <c r="E40" s="2" t="n">
+        <v>44952</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1894,10 +1842,8 @@
       <c r="D41" t="n">
         <v>73937.22</v>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>2017-12-14</t>
-        </is>
+      <c r="E41" s="2" t="n">
+        <v>43083</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -1907,7 +1853,9 @@
       <c r="G41" t="n">
         <v>0.9</v>
       </c>
-      <c r="H41" t="inlineStr"/>
+      <c r="H41" t="b">
+        <v>1</v>
+      </c>
       <c r="I41" t="inlineStr">
         <is>
           <t>On leave</t>
@@ -1929,10 +1877,8 @@
       <c r="D42" t="n">
         <v>84769.33</v>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>2020-08-12</t>
-        </is>
+      <c r="E42" s="2" t="n">
+        <v>44055</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -1968,17 +1914,17 @@
       <c r="D43" t="n">
         <v>73427.37</v>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>2017-01-01</t>
-        </is>
+      <c r="E43" s="2" t="n">
+        <v>42736</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
           <t>HR</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr"/>
+      <c r="G43" t="n">
+        <v>0.68</v>
+      </c>
       <c r="H43" t="b">
         <v>0</v>
       </c>
@@ -2003,10 +1949,8 @@
       <c r="D44" t="n">
         <v>67687.03</v>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>2018/13/01</t>
-        </is>
+      <c r="E44" s="2" t="n">
+        <v>41483</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -2036,20 +1980,16 @@
       <c r="D45" t="n">
         <v>63977.93</v>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>2020-09-10</t>
-        </is>
+      <c r="E45" s="2" t="n">
+        <v>44084</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
           <t>Engineering</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>0.43/1</t>
-        </is>
+      <c r="G45" t="n">
+        <v>0.43</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
@@ -2077,7 +2017,9 @@
       <c r="D46" t="n">
         <v>40429.56</v>
       </c>
-      <c r="E46" t="inlineStr"/>
+      <c r="E46" s="2" t="n">
+        <v>38838</v>
+      </c>
       <c r="F46" t="inlineStr">
         <is>
           <t>HR</t>
@@ -2110,10 +2052,8 @@
       <c r="D47" t="n">
         <v>55603.12</v>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>2016-03-11</t>
-        </is>
+      <c r="E47" s="2" t="n">
+        <v>42440</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -2147,22 +2087,20 @@
       <c r="D48" t="n">
         <v>60787.22</v>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>2022-01-05</t>
-        </is>
+      <c r="E48" s="2" t="n">
+        <v>44566</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
           <t>Engineering</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>0.01/1</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr"/>
+      <c r="G48" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H48" t="b">
+        <v>1</v>
+      </c>
       <c r="I48" t="inlineStr">
         <is>
           <t>Promoted</t>
@@ -2184,10 +2122,8 @@
       <c r="D49" t="n">
         <v>91142.44</v>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>2018-05-07</t>
-        </is>
+      <c r="E49" s="2" t="n">
+        <v>43227</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2197,7 +2133,9 @@
       <c r="G49" t="n">
         <v>0.51</v>
       </c>
-      <c r="H49" t="inlineStr"/>
+      <c r="H49" t="b">
+        <v>1</v>
+      </c>
       <c r="I49" t="inlineStr"/>
     </row>
     <row r="50">
@@ -2215,10 +2153,8 @@
       <c r="D50" t="n">
         <v>76872</v>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>2022-03-02</t>
-        </is>
+      <c r="E50" s="2" t="n">
+        <v>44622</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -2252,10 +2188,8 @@
       <c r="D51" t="n">
         <v>34739.2</v>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>2018/13/01</t>
-        </is>
+      <c r="E51" s="2" t="n">
+        <v>40940</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -2291,10 +2225,8 @@
       <c r="D52" t="n">
         <v>76481.67999999999</v>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>2020-09-10</t>
-        </is>
+      <c r="E52" s="2" t="n">
+        <v>44084</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -2328,10 +2260,8 @@
       <c r="D53" t="n">
         <v>62298.35</v>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>2021-10-30</t>
-        </is>
+      <c r="E53" s="2" t="n">
+        <v>44499</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -2365,10 +2295,8 @@
       <c r="D54" t="n">
         <v>56461.56</v>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>2017-03-25</t>
-        </is>
+      <c r="E54" s="2" t="n">
+        <v>42819</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -2378,7 +2306,9 @@
       <c r="G54" t="n">
         <v>0.9399999999999999</v>
       </c>
-      <c r="H54" t="inlineStr"/>
+      <c r="H54" t="b">
+        <v>1</v>
+      </c>
       <c r="I54" t="inlineStr"/>
     </row>
     <row r="55">
@@ -2396,10 +2326,8 @@
       <c r="D55" t="n">
         <v>82233.53</v>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>2016-09-18</t>
-        </is>
+      <c r="E55" s="2" t="n">
+        <v>42631</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -2435,10 +2363,8 @@
       <c r="D56" t="n">
         <v>90619.99000000001</v>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>2019-03-12</t>
-        </is>
+      <c r="E56" s="2" t="n">
+        <v>43536</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -2448,7 +2374,9 @@
       <c r="G56" t="n">
         <v>0.52</v>
       </c>
-      <c r="H56" t="inlineStr"/>
+      <c r="H56" t="b">
+        <v>0</v>
+      </c>
       <c r="I56" t="inlineStr">
         <is>
           <t>On leave</t>
@@ -2470,18 +2398,20 @@
       <c r="D57" t="n">
         <v>88625</v>
       </c>
-      <c r="E57" t="inlineStr"/>
+      <c r="E57" s="2" t="n">
+        <v>38838</v>
+      </c>
       <c r="F57" t="inlineStr">
         <is>
           <t>Marketing</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>0.7/1</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr"/>
+      <c r="G57" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="H57" t="b">
+        <v>0</v>
+      </c>
       <c r="I57" t="inlineStr"/>
     </row>
     <row r="58">
@@ -2499,10 +2429,8 @@
       <c r="D58" t="n">
         <v>53215.65</v>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>2018/13/01</t>
-        </is>
+      <c r="E58" s="2" t="n">
+        <v>42892</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -2536,10 +2464,8 @@
       <c r="D59" t="n">
         <v>63815.75</v>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>2016-10-23</t>
-        </is>
+      <c r="E59" s="2" t="n">
+        <v>42666</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
@@ -2573,10 +2499,8 @@
       <c r="D60" t="n">
         <v>76625.27</v>
       </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>2021-01-18</t>
-        </is>
+      <c r="E60" s="2" t="n">
+        <v>44214</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -2586,7 +2510,9 @@
       <c r="G60" t="n">
         <v>0.96</v>
       </c>
-      <c r="H60" t="inlineStr"/>
+      <c r="H60" t="b">
+        <v>0</v>
+      </c>
       <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
@@ -2604,10 +2530,8 @@
       <c r="D61" t="n">
         <v>89510.89999999999</v>
       </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>2020-12-12</t>
-        </is>
+      <c r="E61" s="2" t="n">
+        <v>44177</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>

</xml_diff>